<commit_message>
leaving for FULL cellnete at +1_SYNCHRO: 00 Pseudocode
</commit_message>
<xml_diff>
--- a/Pegasus.xlsx
+++ b/Pegasus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\GitHub\T_HUD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9890129C-8E1B-4620-9F8B-FDB933C4470E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{075BBD44-62A4-484A-B555-26BD33BD97AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F8A80F2C-2472-435D-905E-BBF371A10BDB}"/>
   </bookViews>
@@ -292,10 +292,10 @@
     <t>//dreamstime_s_203253415</t>
   </si>
   <si>
-    <t>ILLUSTRATION:</t>
-  </si>
-  <si>
     <t>SOC (e.g. Basement): Parallel Universe Communication Key (PUCK)</t>
+  </si>
+  <si>
+    <t>&lt;= CLICK ILLUSTRATION:</t>
   </si>
 </sst>
 </file>
@@ -1052,14 +1052,14 @@
   <dimension ref="A1:R25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection sqref="A1:M1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="36" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B1" s="37"/>
       <c r="C1" s="37"/>
@@ -1479,8 +1479,8 @@
       <c r="K22" s="8"/>
       <c r="L22" s="8"/>
       <c r="M22" s="17"/>
-      <c r="N22" s="1" t="s">
-        <v>32</v>
+      <c r="N22" s="35" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Readying T_HUD //:sound: Paulina Rubio
</commit_message>
<xml_diff>
--- a/Pegasus.xlsx
+++ b/Pegasus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\GitHub\T_HUD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{075BBD44-62A4-484A-B555-26BD33BD97AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E117ABB7-F8E7-4240-AE7C-67E781C64AD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F8A80F2C-2472-435D-905E-BBF371A10BDB}"/>
   </bookViews>
@@ -295,7 +295,7 @@
     <t>SOC (e.g. Basement): Parallel Universe Communication Key (PUCK)</t>
   </si>
   <si>
-    <t>&lt;= CLICK ILLUSTRATION:</t>
+    <t>&lt;= CLICK ILLUSTRATION after Assigning Macro (see How To):</t>
   </si>
 </sst>
 </file>
@@ -1052,7 +1052,7 @@
   <dimension ref="A1:R25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
successfuly saves as non-macro  //:sound: Richa Sharma, Sukhwinder Singh
</commit_message>
<xml_diff>
--- a/Pegasus.xlsx
+++ b/Pegasus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\GitHub\T_HUD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E117ABB7-F8E7-4240-AE7C-67E781C64AD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{41F65295-D9D7-4D58-BAC9-D9AF2EA6B5E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F8A80F2C-2472-435D-905E-BBF371A10BDB}"/>
   </bookViews>
@@ -1533,7 +1533,8 @@
     <mergeCell ref="A1:M1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>